<commit_message>
Auto commit - 2024-02-04
</commit_message>
<xml_diff>
--- a/2024/2024_02_09_wages/wages_more_info.xlsx
+++ b/2024/2024_02_09_wages/wages_more_info.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="it_wages" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="man_women" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="public_nonpublic" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="source" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="workers_n" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="source" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="52">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -70,6 +72,87 @@
     <t xml:space="preserve">ratio</t>
   </si>
   <si>
+    <t xml:space="preserve">marz_arm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marz_eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workers_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_wage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ք. Երևան</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yerevan city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Արագածոտն</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aragatsotn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Արարատ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ararat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Արմավիր</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armavir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Գեղարքունիք</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gegharkunik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Լոռի</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Կոտայք</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kotayk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Շիրակ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shirak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Սյունիք</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syunik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Վայոց ձոր</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vayots Dzor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Տավուշ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tavush</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.armstat.am/file/article/lab_market_2020_14.pdf</t>
   </si>
   <si>
@@ -80,6 +163,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.armstat.am/file/article/lab_market_2023_14.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ic_employes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ic_wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_employes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not_it_wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_pct</t>
   </si>
 </sst>
 </file>
@@ -304,7 +405,7 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1053,7 +1154,7 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1819,8 +1920,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2583,32 +2684,2716 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F133"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A123" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C133" activeCellId="0" sqref="C133"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>394308</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>201527</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>11898</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>113538</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>26541</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>168027</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>23715</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>135081</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>15879</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>114479</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>26261</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>124293</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>35650</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>137388</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>23220</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>110876</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>22707</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>266832</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>6207</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>126740</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>11851</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>118446</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>101744</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>199037</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>7387</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>111315</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>10310</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>118121</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>12842</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>151143</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>10848</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>122875</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>12734</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>122165</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>11854</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>125680</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>13931</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>117525</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>8925</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>117503</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2867</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>116639</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>6846</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>109507</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>292564</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>202393</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>4510</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>117179</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>16232</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>199725</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>10873</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>116111</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>5031</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>96375</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>13528</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>126296</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>23796</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>143220</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>9288</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>100902</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>13781</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>363545</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>3340</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>135412</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>5005</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>130672</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>417768</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>208044</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>11839</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>119464</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>26808</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>175721</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>24021</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>138167</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>16006</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>121940</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>26197</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>129807</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>35809</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>146076</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>23617</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>117888</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>23371</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>269784</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>6170</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>134099</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>12366</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>122894</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>102931</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>205788</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>7412</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>121048</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>10210</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>128298</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>12775</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>159907</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>10900</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>132700</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>12785</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>129924</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>11593</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>137325</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>13875</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>127588</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>8899</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>130134</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>2815</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>126077</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>6871</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>119293</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>314837</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>208782</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>4426</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>116812</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>16597</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>204895</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>11246</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>113472</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>5106</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>98973</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>13412</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>129696</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>24216</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>150265</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>9742</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>104073</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>14472</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>355654</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>3356</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>140829</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>5496</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>127395</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>440341</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>224815</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>12183</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>125741</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>27327</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>180321</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>24477</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>141190</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>16402</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>125167</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>26819</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>139825</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>35669</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>154056</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>23709</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>123066</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>23645</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>293155</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>6349</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>140988</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>12679</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>125896</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>106696</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>217689</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>7557</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>125687</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>10800</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>132930</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>12937</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>164330</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>11394</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>134821</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>12967</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>136185</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>11752</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>144991</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>13963</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>132869</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>8978</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>137143</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>2912</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>131368</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>6952</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>123629</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>333645</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>227094</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>4626</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>125831</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>16527</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>211290</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>11540</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>115247</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>5008</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>103205</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>13852</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>143232</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>23917</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>158510</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>9746</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>109022</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>14667</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>388656</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>3437</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>149139</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>5727</v>
+      </c>
+      <c r="F100" s="0" t="n">
+        <v>128648</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>471265</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>266164</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>12251</v>
+      </c>
+      <c r="F102" s="0" t="n">
+        <v>132035</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>28051</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <v>193844</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>24970</v>
+      </c>
+      <c r="F104" s="0" t="n">
+        <v>148533</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>16556</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>127949</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>26919</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>137452</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>37170</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>163643</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>24439</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>127381</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>23571</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <v>304540</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>6688</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>153778</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>12903</v>
+      </c>
+      <c r="F111" s="0" t="n">
+        <v>147227</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <v>107039</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>230724</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <v>7572</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>129633</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <v>10975</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>133680</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>12714</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>167233</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <v>11342</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>135762</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <v>12923</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>135901</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <v>11747</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>150667</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <v>14120</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>134669</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <v>9206</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>138711</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <v>2944</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>135636</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <v>7009</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>127263</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E123" s="0" t="n">
+        <v>364226</v>
+      </c>
+      <c r="F123" s="0" t="n">
+        <v>276579</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E124" s="0" t="n">
+        <v>4679</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>135921</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E125" s="0" t="n">
+        <v>17076</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <v>232511</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D126" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E126" s="0" t="n">
+        <v>12256</v>
+      </c>
+      <c r="F126" s="0" t="n">
+        <v>129134</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E127" s="0" t="n">
+        <v>5214</v>
+      </c>
+      <c r="F127" s="0" t="n">
+        <v>110956</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E128" s="0" t="n">
+        <v>13996</v>
+      </c>
+      <c r="F128" s="0" t="n">
+        <v>138885</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <v>25423</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>169638</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D130" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E130" s="0" t="n">
+        <v>10319</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>117407</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E131" s="0" t="n">
+        <v>14365</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>410813</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E132" s="0" t="n">
+        <v>3744</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>168047</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D133" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <v>5894</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>170965</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2625,4 +5410,176 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>21647</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>395163</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>10037</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>566052</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">(C2-E2*G2)/(1-G2)</f>
+        <v>247427.178036176</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">D2/B2</f>
+        <v>0.463667020834296</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>23899</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>434195</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>12076</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>602546</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">(C3-E3*G3)/(1-G3)</f>
+        <v>262241.462319208</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">D3/B3</f>
+        <v>0.505293108498264</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>26716</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>484861</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>14867</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>645225</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">(C4-E4*G4)/(1-G4)</f>
+        <v>283651.481222044</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">D4/B4</f>
+        <v>0.55648300643809</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32329</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>554310</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>20679</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>702614</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">(C5-E5*G5)/(1-G5)</f>
+        <v>291067.21751073</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">D5/B5</f>
+        <v>0.639642426304556</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>40301</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>748235</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>28668</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>917192</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">(C6-E6*G6)/(1-G6)</f>
+        <v>331862.673343076</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">D6/B6</f>
+        <v>0.711347112974864</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>